<commit_message>
horas trabalhadas no maps
</commit_message>
<xml_diff>
--- a/sprints.xlsx
+++ b/sprints.xlsx
@@ -289,7 +289,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -307,6 +306,7 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -663,7 +663,7 @@
   <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -741,7 +741,7 @@
       <c r="I2" s="2">
         <v>1</v>
       </c>
-      <c r="J2" s="20">
+      <c r="J2" s="19">
         <v>42602</v>
       </c>
     </row>
@@ -769,7 +769,7 @@
       <c r="I3" s="2">
         <v>1</v>
       </c>
-      <c r="J3" s="20">
+      <c r="J3" s="19">
         <v>42602</v>
       </c>
     </row>
@@ -829,7 +829,7 @@
       <c r="I5" s="2">
         <v>1</v>
       </c>
-      <c r="J5" s="20">
+      <c r="J5" s="19">
         <v>42602</v>
       </c>
     </row>
@@ -859,7 +859,7 @@
       <c r="I6" s="2">
         <v>1</v>
       </c>
-      <c r="J6" s="20">
+      <c r="J6" s="19">
         <v>42602</v>
       </c>
     </row>
@@ -889,7 +889,7 @@
       <c r="I7" s="2">
         <v>1</v>
       </c>
-      <c r="J7" s="20">
+      <c r="J7" s="19">
         <v>42602</v>
       </c>
     </row>
@@ -953,7 +953,7 @@
       <c r="J9" s="10">
         <v>42616</v>
       </c>
-      <c r="K9" s="14"/>
+      <c r="K9" s="13"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
@@ -971,7 +971,7 @@
       <c r="E10" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F10" s="13"/>
+      <c r="F10" s="20"/>
       <c r="G10" s="1" t="s">
         <v>14</v>
       </c>
@@ -981,10 +981,12 @@
       <c r="I10" s="2">
         <v>0.1</v>
       </c>
-      <c r="J10" s="20">
+      <c r="J10" s="19">
         <v>42616</v>
       </c>
-      <c r="K10" s="13"/>
+      <c r="K10" s="20">
+        <v>8.6111111111111124E-2</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
@@ -1012,7 +1014,7 @@
       <c r="I11" s="2">
         <v>1</v>
       </c>
-      <c r="J11" s="20">
+      <c r="J11" s="19">
         <v>42616</v>
       </c>
     </row>
@@ -1042,7 +1044,7 @@
       <c r="I12" s="2">
         <v>1</v>
       </c>
-      <c r="J12" s="20">
+      <c r="J12" s="19">
         <v>42616</v>
       </c>
     </row>
@@ -1075,7 +1077,7 @@
       <c r="J13" s="10">
         <v>42616</v>
       </c>
-      <c r="K13" s="14"/>
+      <c r="K13" s="13"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
@@ -1121,7 +1123,7 @@
       <c r="D15" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="19" t="s">
+      <c r="E15" s="18" t="s">
         <v>45</v>
       </c>
       <c r="F15" s="7"/>
@@ -1137,7 +1139,7 @@
       <c r="J15" s="10">
         <v>42630</v>
       </c>
-      <c r="K15" s="14"/>
+      <c r="K15" s="13"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
@@ -1199,7 +1201,7 @@
       <c r="J17" s="10">
         <v>42630</v>
       </c>
-      <c r="K17" s="14"/>
+      <c r="K17" s="13"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
@@ -1261,7 +1263,7 @@
       <c r="J19" s="10">
         <v>42630</v>
       </c>
-      <c r="K19" s="14"/>
+      <c r="K19" s="13"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
@@ -1323,7 +1325,7 @@
       <c r="J21" s="10">
         <v>42643</v>
       </c>
-      <c r="K21" s="14"/>
+      <c r="K21" s="13"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
@@ -1385,7 +1387,7 @@
       <c r="J23" s="10">
         <v>42643</v>
       </c>
-      <c r="K23" s="14"/>
+      <c r="K23" s="13"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
@@ -1434,7 +1436,7 @@
       <c r="E25" s="7">
         <v>16</v>
       </c>
-      <c r="F25" s="15"/>
+      <c r="F25" s="14"/>
       <c r="G25" s="7" t="s">
         <v>49</v>
       </c>
@@ -1447,7 +1449,7 @@
       <c r="J25" s="10">
         <v>42658</v>
       </c>
-      <c r="K25" s="14"/>
+      <c r="K25" s="13"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
@@ -1496,7 +1498,7 @@
       <c r="E27" s="7">
         <v>16</v>
       </c>
-      <c r="F27" s="14"/>
+      <c r="F27" s="13"/>
       <c r="G27" s="7" t="s">
         <v>49</v>
       </c>
@@ -1509,7 +1511,7 @@
       <c r="J27" s="10">
         <v>42658</v>
       </c>
-      <c r="K27" s="14"/>
+      <c r="K27" s="13"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
@@ -1541,25 +1543,25 @@
       <c r="K28" s="12"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="16">
+      <c r="A29" s="15">
         <v>28</v>
       </c>
-      <c r="B29" s="17" t="s">
+      <c r="B29" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C29" s="16" t="s">
+      <c r="C29" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="D29" s="16" t="s">
+      <c r="D29" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="E29" s="16"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
-      <c r="H29" s="16"/>
-      <c r="I29" s="17"/>
-      <c r="J29" s="18"/>
-      <c r="K29" s="18"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="17"/>
+      <c r="G29" s="17"/>
+      <c r="H29" s="15"/>
+      <c r="I29" s="16"/>
+      <c r="J29" s="17"/>
+      <c r="K29" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
horas trabalhadas no mapa
</commit_message>
<xml_diff>
--- a/sprints.xlsx
+++ b/sprints.xlsx
@@ -662,8 +662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -985,7 +985,7 @@
         <v>42616</v>
       </c>
       <c r="K10" s="20">
-        <v>8.6111111111111124E-2</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>